<commit_message>
some requirements are added
u
</commit_message>
<xml_diff>
--- a/src/main/java/com/tolgahan/printerbackend/utils/yzc.xlsx
+++ b/src/main/java/com/tolgahan/printerbackend/utils/yzc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mustafa.ozel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Projects\printer-backend\src\main\java\com\tolgahan\printerbackend\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE091EAD-15A9-4F21-BFE8-33D307800499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE2BD2F-DC1E-413E-9C4A-7845807D2218}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="269">
   <si>
     <t>Lokasyon</t>
   </si>
@@ -829,6 +829,9 @@
   </si>
   <si>
     <t>CNMVMBY0TM</t>
+  </si>
+  <si>
+    <t>--------</t>
   </si>
 </sst>
 </file>
@@ -1197,18 +1200,18 @@
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -1244,13 +1247,13 @@
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>159</v>
+        <v>268</v>
       </c>
       <c r="D3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>158</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>168</v>
       </c>
@@ -1306,7 +1309,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>153</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -1348,7 +1351,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -1362,7 +1365,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>173</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>176</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>179</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>182</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>185</v>
       </c>
@@ -1488,7 +1491,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>188</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>194</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>197</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>200</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>206</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>209</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>212</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>218</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>221</v>
       </c>
@@ -1656,7 +1659,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>224</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>227</v>
       </c>
@@ -1684,7 +1687,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>230</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>233</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>236</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -1754,7 +1757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1810,7 +1813,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -2020,7 +2023,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2034,7 +2037,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>77</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -2076,7 +2079,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -2090,7 +2093,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -2104,7 +2107,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>92</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>95</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>98</v>
       </c>
@@ -2146,7 +2149,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>101</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>107</v>
       </c>
@@ -2188,7 +2191,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>110</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>113</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>116</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>119</v>
       </c>
@@ -2244,7 +2247,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>122</v>
       </c>
@@ -2258,7 +2261,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>125</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>25</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>148</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>155</v>
       </c>
@@ -2314,7 +2317,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>150</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>241</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>244</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>247</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>250</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>253</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>256</v>
       </c>
@@ -2412,7 +2415,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>259</v>
       </c>
@@ -2426,7 +2429,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>262</v>
       </c>
@@ -2440,7 +2443,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>265</v>
       </c>

</xml_diff>